<commit_message>
Lacks validation for comment (ish; it's validated, but "no" reponse,BEFIL
</commit_message>
<xml_diff>
--- a/kriterier.xlsx
+++ b/kriterier.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="100">
   <si>
     <t>Applikasjonen er sikret mot SQL injection og XSS.</t>
   </si>
@@ -293,9 +293,6 @@
     <t>Bugs</t>
   </si>
   <si>
-    <t>helpers/posts_helper, metode i Post-modellen</t>
-  </si>
-  <si>
     <t>blog ligger som action i user, så url blir server/users/user_id/blog</t>
   </si>
   <si>
@@ -338,7 +335,10 @@
     <t>controller + model</t>
   </si>
   <si>
-    <t>Migrasjonene er noe rare -- burde brukt references i stedet for å lage foreign keys som integers selv :(</t>
+    <t>partial</t>
+  </si>
+  <si>
+    <t>comments</t>
   </si>
 </sst>
 </file>
@@ -797,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +820,7 @@
         <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -904,27 +904,36 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>97</v>
+        <v>99</v>
+      </c>
+      <c r="C16" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -934,13 +943,13 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
         <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -948,7 +957,7 @@
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -956,7 +965,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -964,15 +973,15 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" t="s">
         <v>86</v>
-      </c>
-      <c r="B23" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1004,7 +1013,7 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1028,11 +1037,11 @@
         <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B32" t="s">
@@ -1040,7 +1049,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B33" t="s">
@@ -1048,7 +1057,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B34" t="s">
@@ -1064,7 +1073,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B36" t="s">
@@ -1072,7 +1081,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B37" t="s">
@@ -1141,11 +1150,11 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B47" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="D47" t="s">
         <v>81</v>
@@ -1157,15 +1166,15 @@
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B51" t="s">
@@ -1173,30 +1182,30 @@
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>95</v>
+      <c r="A53" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="B53" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1225,25 +1234,25 @@
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="5" t="s">
         <v>74</v>
       </c>
       <c r="B62" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="5" t="s">
         <v>76</v>
       </c>
       <c r="B64" t="s">
@@ -1251,9 +1260,7 @@
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
-        <v>99</v>
-      </c>
+      <c r="A67" s="7"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">

</xml_diff>